<commit_message>
Changes to framework - added ExtentReport class, updated comments
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Case_Data_Maps.xlsx
+++ b/src/test/resources/Test_Case_Data_Maps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tm0338\eclipse-workspace\UIAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2375C8FA-CD35-4E17-B02E-813827E89F4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43672495-F149-453D-B6E3-ED10B71751E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6C7B5E75-A1B0-44CC-8594-A37FB5E291D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6C7B5E75-A1B0-44CC-8594-A37FB5E291D1}"/>
   </bookViews>
   <sheets>
     <sheet name="ElementMap" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="82">
   <si>
     <t>Page</t>
   </si>
@@ -262,7 +262,22 @@
     <t>Test_Case_Name</t>
   </si>
   <si>
-    <t>BuyAllTshirtsTest</t>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>btn_mainMenu</t>
+  </si>
+  <si>
+    <t>div#menu_button_container  &gt; button</t>
+  </si>
+  <si>
+    <t>lnk_productsMenuLink</t>
+  </si>
+  <si>
+    <t>inventory_sidebar_link</t>
+  </si>
+  <si>
+    <t>buyAllTshirtsTest</t>
   </si>
 </sst>
 </file>
@@ -659,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5E13B9-B6B9-4D43-9548-D0513821EDDA}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,53 +759,53 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -798,16 +813,16 @@
         <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -815,16 +830,16 @@
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -832,16 +847,16 @@
         <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -849,50 +864,50 @@
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -900,50 +915,50 @@
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,16 +966,16 @@
         <v>34</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -968,16 +983,16 @@
         <v>34</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -988,13 +1003,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1002,50 +1017,50 @@
         <v>34</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,49 +1068,83 @@
         <v>44</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="5" t="s">
+      <c r="D26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1109,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8DC2494-81A6-473D-A102-26E292889F4E}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,7 +1190,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>71</v>
@@ -1158,5 +1207,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>